<commit_message>
Adicion de cambios menores
Se ingresa cuadro actulizado y se actuliza varios pormenores
</commit_message>
<xml_diff>
--- a/Sprint Backlog_full.xlsx
+++ b/Sprint Backlog_full.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\OneDrive\Documentos\GitHub\Proyecto_7mo_Ing.Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Historias de Usuario'!$B:$G,'Historias de Usuario'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -450,7 +450,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -972,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1054,24 +1054,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1170,12 +1152,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1210,16 +1186,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,11 +1530,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="5" topLeftCell="H35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="7" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42:S42"/>
+      <selection pane="bottomRight" activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,9 +1543,9 @@
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="92" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="92" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1625,295 +1628,295 @@
       </c>
     </row>
     <row r="4" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I4" s="72" t="s">
+      <c r="I4" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="72" t="s">
+      <c r="J4" s="91"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="73"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="72" t="s">
+      <c r="M4" s="91"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="72" t="s">
+      <c r="P4" s="91"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="73"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="72" t="s">
+      <c r="S4" s="91"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="73"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="72" t="s">
+      <c r="V4" s="91"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="72" t="s">
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="72" t="s">
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="72" t="s">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="72" t="s">
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="72" t="s">
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="72" t="s">
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="AQ4" s="73"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="72" t="s">
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="72" t="s">
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="72" t="s">
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="66"/>
+      <c r="AY4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="72" t="s">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="66"/>
+      <c r="BB4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="72" t="s">
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="66"/>
+      <c r="BE4" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="74"/>
-      <c r="BH4" s="72" t="s">
+      <c r="BF4" s="91"/>
+      <c r="BG4" s="66"/>
+      <c r="BH4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="74"/>
-      <c r="BK4" s="72" t="s">
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="66"/>
+      <c r="BK4" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="BL4" s="73"/>
-      <c r="BM4" s="74"/>
-      <c r="BN4" s="72" t="s">
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="66"/>
+      <c r="BN4" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="74"/>
-      <c r="BQ4" s="72" t="s">
+      <c r="BO4" s="91"/>
+      <c r="BP4" s="66"/>
+      <c r="BQ4" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="BR4" s="73"/>
+      <c r="BR4" s="91"/>
     </row>
     <row r="5" spans="2:71" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="78" t="s">
+      <c r="F5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78" t="s">
+      <c r="J5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78" t="s">
+      <c r="M5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78" t="s">
+      <c r="P5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78" t="s">
+      <c r="S5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="V5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78" t="s">
+      <c r="V5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="Y5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78" t="s">
+      <c r="Y5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78" t="s">
+      <c r="AB5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC5" s="70"/>
+      <c r="AD5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AE5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78" t="s">
+      <c r="AE5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="70"/>
+      <c r="AG5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AH5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78" t="s">
+      <c r="AH5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" s="70"/>
+      <c r="AJ5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AK5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78" t="s">
+      <c r="AK5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL5" s="70"/>
+      <c r="AM5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AN5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78" t="s">
+      <c r="AN5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO5" s="70"/>
+      <c r="AP5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AQ5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78" t="s">
+      <c r="AQ5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR5" s="70"/>
+      <c r="AS5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AT5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78" t="s">
+      <c r="AT5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU5" s="70"/>
+      <c r="AV5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AW5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78" t="s">
+      <c r="AW5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX5" s="70"/>
+      <c r="AY5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AZ5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78" t="s">
+      <c r="AZ5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA5" s="70"/>
+      <c r="BB5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BC5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="78" t="s">
+      <c r="BC5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BF5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="78" t="s">
+      <c r="BF5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG5" s="70"/>
+      <c r="BH5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BI5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BJ5" s="78"/>
-      <c r="BK5" s="78" t="s">
+      <c r="BI5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ5" s="70"/>
+      <c r="BK5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BL5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BM5" s="78"/>
-      <c r="BN5" s="78" t="s">
+      <c r="BL5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM5" s="70"/>
+      <c r="BN5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BO5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BP5" s="78"/>
-      <c r="BQ5" s="78" t="s">
+      <c r="BO5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BP5" s="70"/>
+      <c r="BQ5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BR5" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="BS5" s="79"/>
+      <c r="BR5" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="BS5" s="71"/>
     </row>
-    <row r="6" spans="2:71" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+    <row r="6" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="85" t="s">
         <v>51</v>
       </c>
       <c r="G6" s="25" t="s">
@@ -1922,34 +1925,34 @@
       <c r="H6" s="14">
         <v>4</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="45">
         <v>4</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="45">
         <f>H6-I6</f>
         <v>0</v>
       </c>
-      <c r="K6" s="44"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50">
+      <c r="K6" s="38"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44">
         <f t="shared" ref="M6:M23" si="0">J6-L6</f>
         <v>0</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50">
+      <c r="O6" s="44"/>
+      <c r="P6" s="44">
         <f t="shared" ref="P6:P23" si="1">M6-O6</f>
         <v>0</v>
       </c>
       <c r="Q6" s="16"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50">
+      <c r="R6" s="44"/>
+      <c r="S6" s="44">
         <f t="shared" ref="S6:S23" si="2">P6-R6</f>
         <v>0</v>
       </c>
       <c r="T6" s="16"/>
-      <c r="U6" s="50"/>
-      <c r="V6" s="50">
+      <c r="U6" s="44"/>
+      <c r="V6" s="44">
         <f t="shared" ref="V6:V23" si="3">S6-U6</f>
         <v>0</v>
       </c>
@@ -2055,15 +2058,15 @@
       <c r="BS6" s="30"/>
     </row>
     <row r="7" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="66" t="s">
+      <c r="B7" s="83"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="25" t="s">
         <v>53</v>
       </c>
@@ -2076,28 +2079,28 @@
         <v>3</v>
       </c>
       <c r="K7" s="7"/>
-      <c r="L7" s="52">
+      <c r="L7" s="46">
         <v>3</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="45"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48">
+      <c r="N7" s="39"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q7" s="7"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48">
+      <c r="R7" s="42"/>
+      <c r="S7" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T7" s="7"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48">
+      <c r="U7" s="42"/>
+      <c r="V7" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2202,16 +2205,16 @@
       </c>
       <c r="BS7" s="31"/>
     </row>
-    <row r="8" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="66" t="s">
+    <row r="8" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="83"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="86"/>
       <c r="G8" s="25" t="s">
         <v>53</v>
       </c>
@@ -2224,30 +2227,30 @@
         <v>5</v>
       </c>
       <c r="K8" s="7"/>
-      <c r="L8" s="52">
+      <c r="L8" s="46">
         <v>3</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="46">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N8" s="7"/>
-      <c r="O8" s="52">
-        <v>2</v>
-      </c>
-      <c r="P8" s="52">
+      <c r="O8" s="46">
+        <v>2</v>
+      </c>
+      <c r="P8" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48">
+      <c r="Q8" s="39"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T8" s="7"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48">
+      <c r="U8" s="42"/>
+      <c r="V8" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2353,15 +2356,15 @@
       <c r="BS8" s="31"/>
     </row>
     <row r="9" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="66" t="s">
+      <c r="B9" s="83"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="25" t="s">
         <v>53</v>
       </c>
@@ -2380,30 +2383,30 @@
         <v>8</v>
       </c>
       <c r="N9" s="7"/>
-      <c r="O9" s="52">
+      <c r="O9" s="46">
         <v>4</v>
       </c>
-      <c r="P9" s="52">
+      <c r="P9" s="46">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q9" s="7"/>
-      <c r="R9" s="52">
-        <v>2</v>
-      </c>
-      <c r="S9" s="52">
+      <c r="R9" s="46">
+        <v>2</v>
+      </c>
+      <c r="S9" s="46">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="T9" s="45"/>
-      <c r="U9" s="53"/>
-      <c r="V9" s="53">
+      <c r="T9" s="39"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W9" s="7"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="48">
+      <c r="X9" s="42"/>
+      <c r="Y9" s="42">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -2503,16 +2506,16 @@
       <c r="BS9" s="31"/>
     </row>
     <row r="10" spans="2:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="35"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="70" t="s">
+      <c r="B10" s="84"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="80" t="s">
+      <c r="F10" s="87"/>
+      <c r="G10" s="72" t="s">
         <v>53</v>
       </c>
       <c r="H10" s="20">
@@ -2531,7 +2534,7 @@
       </c>
       <c r="N10" s="22"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="49">
+      <c r="P10" s="43">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -2563,9 +2566,9 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="43"/>
-      <c r="AE10" s="43">
+      <c r="AC10" s="40"/>
+      <c r="AD10" s="37"/>
+      <c r="AE10" s="37">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -2646,20 +2649,20 @@
       <c r="BR10" s="24"/>
       <c r="BS10" s="32"/>
     </row>
-    <row r="11" spans="2:71" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="85" t="s">
         <v>57</v>
       </c>
       <c r="G11" s="25" t="s">
@@ -2668,34 +2671,34 @@
       <c r="H11" s="14">
         <v>4</v>
       </c>
-      <c r="I11" s="51">
+      <c r="I11" s="45">
         <v>4</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="45">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K11" s="44"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50">
+      <c r="K11" s="38"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" s="16"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50">
+      <c r="O11" s="44"/>
+      <c r="P11" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q11" s="16"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50">
+      <c r="R11" s="44"/>
+      <c r="S11" s="44">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T11" s="16"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50">
+      <c r="U11" s="44"/>
+      <c r="V11" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2801,49 +2804,49 @@
       <c r="BS11" s="30"/>
     </row>
     <row r="12" spans="2:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="66" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="37"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="H12" s="5">
         <v>3</v>
       </c>
-      <c r="I12" s="48"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="6">
         <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="K12" s="7"/>
-      <c r="L12" s="52">
+      <c r="L12" s="46">
         <v>3</v>
       </c>
-      <c r="M12" s="52">
+      <c r="M12" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="45"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48">
+      <c r="N12" s="39"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q12" s="7"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48">
+      <c r="R12" s="42"/>
+      <c r="S12" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T12" s="7"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48">
+      <c r="U12" s="42"/>
+      <c r="V12" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2948,54 +2951,54 @@
       </c>
       <c r="BS12" s="31"/>
     </row>
-    <row r="13" spans="2:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="66" t="s">
+    <row r="13" spans="2:71" x14ac:dyDescent="0.25">
+      <c r="B13" s="83"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="37"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="25" t="s">
         <v>53</v>
       </c>
       <c r="H13" s="5">
         <v>5</v>
       </c>
-      <c r="I13" s="48"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="6">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="K13" s="7"/>
-      <c r="L13" s="52">
-        <v>2</v>
-      </c>
-      <c r="M13" s="52">
+      <c r="L13" s="46">
+        <v>2</v>
+      </c>
+      <c r="M13" s="46">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N13" s="7"/>
-      <c r="O13" s="52">
+      <c r="O13" s="46">
         <v>3</v>
       </c>
-      <c r="P13" s="52">
+      <c r="P13" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q13" s="7"/>
-      <c r="R13" s="48">
-        <v>1</v>
-      </c>
-      <c r="S13" s="48">
+      <c r="R13" s="42">
+        <v>1</v>
+      </c>
+      <c r="S13" s="42">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="T13" s="45"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="54">
+      <c r="T13" s="39"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -3100,17 +3103,17 @@
       </c>
       <c r="BS13" s="31"/>
     </row>
-    <row r="14" spans="2:71" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="66" t="s">
+    <row r="14" spans="2:71" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="83"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="39" t="s">
+      <c r="F14" s="86"/>
+      <c r="G14" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="5">
@@ -3128,18 +3131,18 @@
         <v>12</v>
       </c>
       <c r="N14" s="7"/>
-      <c r="O14" s="52">
-        <v>2</v>
-      </c>
-      <c r="P14" s="52">
+      <c r="O14" s="46">
+        <v>2</v>
+      </c>
+      <c r="P14" s="46">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Q14" s="7"/>
-      <c r="R14" s="52">
+      <c r="R14" s="46">
         <v>4</v>
       </c>
-      <c r="S14" s="52">
+      <c r="S14" s="46">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -3244,17 +3247,17 @@
       <c r="BR14" s="8"/>
       <c r="BS14" s="31"/>
     </row>
-    <row r="15" spans="2:71" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="66" t="s">
+    <row r="15" spans="2:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="83"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="40" t="s">
+      <c r="F15" s="86"/>
+      <c r="G15" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H15" s="5">
@@ -3384,17 +3387,17 @@
       <c r="BR15" s="8"/>
       <c r="BS15" s="31"/>
     </row>
-    <row r="16" spans="2:71" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="66" t="s">
+    <row r="16" spans="2:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="83"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="39" t="s">
+      <c r="F16" s="86"/>
+      <c r="G16" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H16" s="26">
@@ -3417,32 +3420,32 @@
         <v>6</v>
       </c>
       <c r="Q16" s="28"/>
-      <c r="R16" s="56">
-        <v>2</v>
-      </c>
-      <c r="S16" s="56">
+      <c r="R16" s="50">
+        <v>2</v>
+      </c>
+      <c r="S16" s="50">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="T16" s="28"/>
-      <c r="U16" s="56">
+      <c r="U16" s="50">
         <v>4</v>
       </c>
-      <c r="V16" s="56">
+      <c r="V16" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W16" s="28"/>
-      <c r="X16" s="56">
-        <v>2</v>
-      </c>
-      <c r="Y16" s="56">
+      <c r="X16" s="50">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="50">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="58"/>
-      <c r="AB16" s="58">
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="52"/>
+      <c r="AB16" s="52">
         <f t="shared" si="5"/>
         <v>-2</v>
       </c>
@@ -3530,16 +3533,16 @@
       <c r="BS16" s="31"/>
     </row>
     <row r="17" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="70" t="s">
+      <c r="B17" s="84"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="71" t="s">
+      <c r="F17" s="87"/>
+      <c r="G17" s="65" t="s">
         <v>63</v>
       </c>
       <c r="H17" s="20">
@@ -3675,20 +3678,20 @@
       </c>
       <c r="BS17" s="32"/>
     </row>
-    <row r="18" spans="1:71" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+    <row r="18" spans="1:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="85" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="25" t="s">
@@ -3697,14 +3700,14 @@
       <c r="H18" s="14">
         <v>4</v>
       </c>
-      <c r="I18" s="51">
+      <c r="I18" s="45">
         <v>4</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="45">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K18" s="44"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15">
         <f t="shared" si="0"/>
@@ -3830,31 +3833,31 @@
       <c r="BS18" s="30"/>
     </row>
     <row r="19" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="66" t="s">
+      <c r="B19" s="83"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="37"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="25" t="s">
         <v>53</v>
       </c>
       <c r="H19" s="5">
         <v>3</v>
       </c>
-      <c r="I19" s="52">
-        <v>2</v>
-      </c>
-      <c r="J19" s="52">
+      <c r="I19" s="46">
+        <v>2</v>
+      </c>
+      <c r="J19" s="46">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53">
+      <c r="K19" s="39"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3977,17 +3980,17 @@
       </c>
       <c r="BS19" s="31"/>
     </row>
-    <row r="20" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="66" t="s">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B20" s="83"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="39" t="s">
+      <c r="F20" s="86"/>
+      <c r="G20" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H20" s="5">
@@ -3999,22 +4002,22 @@
         <v>5</v>
       </c>
       <c r="K20" s="7"/>
-      <c r="L20" s="52">
+      <c r="L20" s="46">
         <v>3</v>
       </c>
-      <c r="M20" s="52">
+      <c r="M20" s="46">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N20" s="7"/>
-      <c r="O20" s="52">
-        <v>2</v>
-      </c>
-      <c r="P20" s="52">
+      <c r="O20" s="46">
+        <v>2</v>
+      </c>
+      <c r="P20" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="45"/>
+      <c r="Q20" s="39"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6">
         <f t="shared" si="2"/>
@@ -4127,17 +4130,17 @@
       </c>
       <c r="BS20" s="31"/>
     </row>
-    <row r="21" spans="1:71" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="66" t="s">
+    <row r="21" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="83"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="40" t="s">
+      <c r="F21" s="86"/>
+      <c r="G21" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H21" s="26">
@@ -4264,20 +4267,20 @@
       </c>
       <c r="BP21" s="28"/>
       <c r="BQ21" s="29"/>
-      <c r="BR21" s="41"/>
+      <c r="BR21" s="35"/>
       <c r="BS21" s="31"/>
     </row>
-    <row r="22" spans="1:71" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="66" t="s">
+    <row r="22" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="83"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="40" t="s">
+      <c r="F22" s="86"/>
+      <c r="G22" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="26">
@@ -4404,20 +4407,20 @@
       </c>
       <c r="BP22" s="28"/>
       <c r="BQ22" s="29"/>
-      <c r="BR22" s="41"/>
+      <c r="BR22" s="35"/>
       <c r="BS22" s="31"/>
     </row>
     <row r="23" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="35"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="70" t="s">
+      <c r="B23" s="84"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="81" t="s">
+      <c r="F23" s="87"/>
+      <c r="G23" s="73" t="s">
         <v>62</v>
       </c>
       <c r="H23" s="20">
@@ -4429,32 +4432,32 @@
         <v>6</v>
       </c>
       <c r="K23" s="22"/>
-      <c r="L23" s="59">
-        <v>2</v>
-      </c>
-      <c r="M23" s="59">
+      <c r="L23" s="53">
+        <v>2</v>
+      </c>
+      <c r="M23" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="N23" s="22"/>
-      <c r="O23" s="59">
+      <c r="O23" s="53">
         <v>3</v>
       </c>
-      <c r="P23" s="59">
+      <c r="P23" s="53">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q23" s="22"/>
-      <c r="R23" s="59">
-        <v>2</v>
-      </c>
-      <c r="S23" s="59">
+      <c r="R23" s="53">
+        <v>2</v>
+      </c>
+      <c r="S23" s="53">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="T23" s="46"/>
-      <c r="U23" s="60"/>
-      <c r="V23" s="60">
+      <c r="T23" s="40"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="54">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -4559,23 +4562,23 @@
       </c>
       <c r="BS23" s="32"/>
     </row>
-    <row r="24" spans="1:71" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
+    <row r="24" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="64" t="s">
+      <c r="E24" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="76" t="s">
+      <c r="G24" s="68" t="s">
         <v>53</v>
       </c>
       <c r="H24" s="10">
@@ -4617,14 +4620,14 @@
         <v>4</v>
       </c>
       <c r="Z24" s="12"/>
-      <c r="AA24" s="55">
+      <c r="AA24" s="49">
         <v>4</v>
       </c>
-      <c r="AB24" s="55">
+      <c r="AB24" s="49">
         <f t="shared" ref="AB24:AB29" si="28">Y24-AA24</f>
         <v>0</v>
       </c>
-      <c r="AC24" s="47"/>
+      <c r="AC24" s="41"/>
       <c r="AD24" s="11"/>
       <c r="AE24" s="11">
         <f t="shared" ref="AE24:AE29" si="29">AB24-AD24</f>
@@ -4714,16 +4717,16 @@
       <c r="BS24" s="31"/>
     </row>
     <row r="25" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="66" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="39" t="s">
+      <c r="F25" s="86"/>
+      <c r="G25" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H25" s="5">
@@ -4765,22 +4768,22 @@
         <v>3</v>
       </c>
       <c r="Z25" s="7"/>
-      <c r="AA25" s="52">
-        <v>1</v>
-      </c>
-      <c r="AB25" s="52">
+      <c r="AA25" s="46">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="46">
         <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="AC25" s="7"/>
-      <c r="AD25" s="52">
-        <v>2</v>
-      </c>
-      <c r="AE25" s="52">
+      <c r="AD25" s="46">
+        <v>2</v>
+      </c>
+      <c r="AE25" s="46">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AF25" s="45"/>
+      <c r="AF25" s="39"/>
       <c r="AG25" s="6"/>
       <c r="AH25" s="6">
         <f t="shared" si="30"/>
@@ -4863,17 +4866,17 @@
       </c>
       <c r="BS25" s="31"/>
     </row>
-    <row r="26" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="34"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="66" t="s">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="B26" s="83"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="39" t="s">
+      <c r="F26" s="86"/>
+      <c r="G26" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H26" s="5">
@@ -4921,24 +4924,24 @@
         <v>5</v>
       </c>
       <c r="AC26" s="7"/>
-      <c r="AD26" s="52">
+      <c r="AD26" s="46">
         <v>3</v>
       </c>
-      <c r="AE26" s="52">
+      <c r="AE26" s="46">
         <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="AF26" s="7"/>
-      <c r="AG26" s="52">
-        <v>1</v>
-      </c>
-      <c r="AH26" s="52">
+      <c r="AG26" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="46">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="AI26" s="45"/>
-      <c r="AJ26" s="53"/>
-      <c r="AK26" s="53">
+      <c r="AI26" s="39"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
@@ -5013,17 +5016,17 @@
       </c>
       <c r="BS26" s="31"/>
     </row>
-    <row r="27" spans="1:71" ht="45" x14ac:dyDescent="0.25">
-      <c r="B27" s="34"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="66" t="s">
+    <row r="27" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="83"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="40" t="s">
+      <c r="F27" s="86"/>
+      <c r="G27" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H27" s="26">
@@ -5154,16 +5157,16 @@
       <c r="BS27" s="31"/>
     </row>
     <row r="28" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="66" t="s">
+      <c r="B28" s="83"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="65" t="s">
+      <c r="E28" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="40" t="s">
+      <c r="F28" s="86"/>
+      <c r="G28" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="26">
@@ -5294,16 +5297,16 @@
       <c r="BS28" s="31"/>
     </row>
     <row r="29" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="67" t="s">
+      <c r="B29" s="83"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E29" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="39" t="s">
+      <c r="F29" s="86"/>
+      <c r="G29" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H29" s="26">
@@ -5357,24 +5360,24 @@
         <v>8</v>
       </c>
       <c r="AF29" s="28"/>
-      <c r="AG29" s="56">
+      <c r="AG29" s="50">
         <v>4</v>
       </c>
-      <c r="AH29" s="56">
+      <c r="AH29" s="50">
         <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="AI29" s="28"/>
-      <c r="AJ29" s="56">
+      <c r="AJ29" s="50">
         <v>3</v>
       </c>
-      <c r="AK29" s="56">
+      <c r="AK29" s="50">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
-      <c r="AL29" s="57"/>
-      <c r="AM29" s="82"/>
-      <c r="AN29" s="82">
+      <c r="AL29" s="51"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="74">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
@@ -5444,20 +5447,20 @@
       <c r="BS29" s="31"/>
     </row>
     <row r="30" spans="1:71" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33" t="s">
+      <c r="A30" s="82"/>
+      <c r="B30" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="61" t="s">
+      <c r="E30" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="36" t="s">
+      <c r="F30" s="85" t="s">
         <v>51</v>
       </c>
       <c r="G30" s="25" t="s">
@@ -5468,148 +5471,148 @@
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="15">
-        <f t="shared" ref="J30:J34" si="44">H30-I30</f>
+        <f t="shared" ref="J30:J33" si="44">H30-I30</f>
         <v>4</v>
       </c>
       <c r="K30" s="16"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15">
-        <f t="shared" ref="M30:M34" si="45">J30-L30</f>
+        <f t="shared" ref="M30:M33" si="45">J30-L30</f>
         <v>4</v>
       </c>
       <c r="N30" s="16"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15">
-        <f t="shared" ref="P30:P34" si="46">M30-O30</f>
+        <f t="shared" ref="P30:P33" si="46">M30-O30</f>
         <v>4</v>
       </c>
       <c r="Q30" s="16"/>
       <c r="R30" s="15"/>
       <c r="S30" s="15">
-        <f t="shared" ref="S30:S34" si="47">P30-R30</f>
+        <f t="shared" ref="S30:S33" si="47">P30-R30</f>
         <v>4</v>
       </c>
       <c r="T30" s="16"/>
       <c r="U30" s="15"/>
       <c r="V30" s="15">
-        <f t="shared" ref="V30:V34" si="48">S30-U30</f>
+        <f t="shared" ref="V30:V33" si="48">S30-U30</f>
         <v>4</v>
       </c>
       <c r="W30" s="16"/>
-      <c r="X30" s="51">
+      <c r="X30" s="45">
         <v>4</v>
       </c>
-      <c r="Y30" s="51">
-        <f t="shared" ref="Y30:Y34" si="49">V30-X30</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="44"/>
+      <c r="Y30" s="45">
+        <f t="shared" ref="Y30:Y33" si="49">V30-X30</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="38"/>
       <c r="AA30" s="15"/>
       <c r="AB30" s="15">
-        <f t="shared" ref="AB30:AB34" si="50">Y30-AA30</f>
+        <f t="shared" ref="AB30:AB33" si="50">Y30-AA30</f>
         <v>0</v>
       </c>
       <c r="AC30" s="16"/>
       <c r="AD30" s="15"/>
       <c r="AE30" s="15">
-        <f t="shared" ref="AE30:AE34" si="51">AB30-AD30</f>
+        <f t="shared" ref="AE30:AE33" si="51">AB30-AD30</f>
         <v>0</v>
       </c>
       <c r="AF30" s="16"/>
       <c r="AG30" s="15"/>
       <c r="AH30" s="15">
-        <f t="shared" ref="AH30:AH34" si="52">AE30-AG30</f>
+        <f t="shared" ref="AH30:AH33" si="52">AE30-AG30</f>
         <v>0</v>
       </c>
       <c r="AI30" s="16"/>
       <c r="AJ30" s="15"/>
       <c r="AK30" s="15">
-        <f t="shared" ref="AK30:AK34" si="53">AH30-AJ30</f>
+        <f t="shared" ref="AK30:AK33" si="53">AH30-AJ30</f>
         <v>0</v>
       </c>
       <c r="AL30" s="16"/>
       <c r="AM30" s="15"/>
       <c r="AN30" s="15">
-        <f t="shared" ref="AN30:AN34" si="54">AK30-AM30</f>
+        <f t="shared" ref="AN30:AN33" si="54">AK30-AM30</f>
         <v>0</v>
       </c>
       <c r="AO30" s="16"/>
       <c r="AP30" s="15"/>
       <c r="AQ30" s="15">
-        <f t="shared" ref="AQ30:AQ34" si="55">AN30-AP30</f>
+        <f t="shared" ref="AQ30:AQ33" si="55">AN30-AP30</f>
         <v>0</v>
       </c>
       <c r="AR30" s="16"/>
       <c r="AS30" s="15"/>
       <c r="AT30" s="15">
-        <f t="shared" ref="AT30:AT34" si="56">AQ30-AS30</f>
+        <f t="shared" ref="AT30:AT33" si="56">AQ30-AS30</f>
         <v>0</v>
       </c>
       <c r="AU30" s="16"/>
       <c r="AV30" s="15"/>
       <c r="AW30" s="15">
-        <f t="shared" ref="AW30:AW34" si="57">AT30-AV30</f>
+        <f t="shared" ref="AW30:AW33" si="57">AT30-AV30</f>
         <v>0</v>
       </c>
       <c r="AX30" s="16"/>
       <c r="AY30" s="15"/>
       <c r="AZ30" s="15">
-        <f t="shared" ref="AZ30:AZ34" si="58">AW30-AY30</f>
+        <f t="shared" ref="AZ30:AZ33" si="58">AW30-AY30</f>
         <v>0</v>
       </c>
       <c r="BA30" s="16"/>
       <c r="BB30" s="15"/>
       <c r="BC30" s="15">
-        <f t="shared" ref="BC30:BC34" si="59">AZ30-BB30</f>
+        <f t="shared" ref="BC30:BC33" si="59">AZ30-BB30</f>
         <v>0</v>
       </c>
       <c r="BD30" s="16"/>
       <c r="BE30" s="15"/>
       <c r="BF30" s="15">
-        <f t="shared" ref="BF30:BF34" si="60">BC30-BE30</f>
+        <f t="shared" ref="BF30:BF33" si="60">BC30-BE30</f>
         <v>0</v>
       </c>
       <c r="BG30" s="16"/>
       <c r="BH30" s="15"/>
       <c r="BI30" s="15">
-        <f t="shared" ref="BI30:BI34" si="61">BF30-BH30</f>
+        <f t="shared" ref="BI30:BI33" si="61">BF30-BH30</f>
         <v>0</v>
       </c>
       <c r="BJ30" s="16"/>
       <c r="BK30" s="15"/>
       <c r="BL30" s="15">
-        <f t="shared" ref="BL30:BL34" si="62">BI30-BK30</f>
+        <f t="shared" ref="BL30:BL33" si="62">BI30-BK30</f>
         <v>0</v>
       </c>
       <c r="BM30" s="16"/>
       <c r="BN30" s="15"/>
       <c r="BO30" s="15">
-        <f t="shared" ref="BO30:BO34" si="63">BL30-BN30</f>
+        <f t="shared" ref="BO30:BO33" si="63">BL30-BN30</f>
         <v>0</v>
       </c>
       <c r="BP30" s="16"/>
       <c r="BQ30" s="17">
-        <f t="shared" ref="BQ30:BQ34" si="64">I30+L30+O30+R30+U30+X30+AA30+AD30+AG30+AJ30+AM30+AP30+AS30+AV30+AY30+BB30+BE30+BH30+BK30+BN30</f>
+        <f t="shared" ref="BQ30:BQ32" si="64">I30+L30+O30+R30+U30+X30+AA30+AD30+AG30+AJ30+AM30+AP30+AS30+AV30+AY30+BB30+BE30+BH30+BK30+BN30</f>
         <v>4</v>
       </c>
       <c r="BR30" s="17">
-        <f t="shared" ref="BR30:BR34" si="65">H30-BQ30</f>
+        <f t="shared" ref="BR30:BR32" si="65">H30-BQ30</f>
         <v>0</v>
       </c>
       <c r="BS30" s="30"/>
     </row>
     <row r="31" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="66" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="39" t="s">
+      <c r="F31" s="86"/>
+      <c r="G31" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H31" s="5">
@@ -5645,10 +5648,10 @@
         <v>3</v>
       </c>
       <c r="W31" s="7"/>
-      <c r="X31" s="52">
-        <v>2</v>
-      </c>
-      <c r="Y31" s="52">
+      <c r="X31" s="46">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="46">
         <f t="shared" si="49"/>
         <v>1</v>
       </c>
@@ -5747,18 +5750,18 @@
       </c>
       <c r="BS31" s="31"/>
     </row>
-    <row r="32" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="66" t="s">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A32" s="83"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="39" t="s">
+      <c r="F32" s="86"/>
+      <c r="G32" s="33" t="s">
         <v>62</v>
       </c>
       <c r="H32" s="5">
@@ -5800,10 +5803,10 @@
         <v>5</v>
       </c>
       <c r="Z32" s="7"/>
-      <c r="AA32" s="52">
-        <v>2</v>
-      </c>
-      <c r="AB32" s="52">
+      <c r="AA32" s="46">
+        <v>2</v>
+      </c>
+      <c r="AB32" s="46">
         <f t="shared" si="50"/>
         <v>3</v>
       </c>
@@ -5897,17 +5900,17 @@
       <c r="BS32" s="31"/>
     </row>
     <row r="33" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="66" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="65" t="s">
+      <c r="E33" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="40" t="s">
+      <c r="F33" s="86"/>
+      <c r="G33" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H33" s="26">
@@ -6038,17 +6041,17 @@
       <c r="BS33" s="31"/>
     </row>
     <row r="34" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="35"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="70" t="s">
+      <c r="A34" s="84"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="38"/>
-      <c r="G34" s="81" t="s">
+      <c r="F34" s="87"/>
+      <c r="G34" s="73" t="s">
         <v>62</v>
       </c>
       <c r="H34" s="20">
@@ -6090,10 +6093,10 @@
         <v>8</v>
       </c>
       <c r="Z34" s="22"/>
-      <c r="AA34" s="59">
+      <c r="AA34" s="53">
         <v>3</v>
       </c>
-      <c r="AB34" s="59">
+      <c r="AB34" s="53">
         <f t="shared" ref="AB34:AB37" si="72">Y34-AA34</f>
         <v>5</v>
       </c>
@@ -6186,23 +6189,23 @@
       </c>
       <c r="BS34" s="32"/>
     </row>
-    <row r="35" spans="1:71" ht="60" x14ac:dyDescent="0.25">
-      <c r="B35" s="33" t="s">
+    <row r="35" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G35" s="69" t="s">
+      <c r="G35" s="63" t="s">
         <v>63</v>
       </c>
       <c r="H35" s="14">
@@ -6339,16 +6342,16 @@
       <c r="BS35" s="30"/>
     </row>
     <row r="36" spans="1:71" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="66" t="s">
+      <c r="B36" s="83"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="40" t="s">
+      <c r="F36" s="86"/>
+      <c r="G36" s="34" t="s">
         <v>63</v>
       </c>
       <c r="H36" s="5">
@@ -6484,17 +6487,17 @@
       </c>
       <c r="BS36" s="31"/>
     </row>
-    <row r="37" spans="1:71" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="35"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="70" t="s">
+    <row r="37" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="84"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="63" t="s">
+      <c r="E37" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="71" t="s">
+      <c r="F37" s="87"/>
+      <c r="G37" s="65" t="s">
         <v>63</v>
       </c>
       <c r="H37" s="20">
@@ -6634,110 +6637,109 @@
       <c r="B39" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="87" t="s">
+      <c r="C39" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="83"/>
-      <c r="E39" s="90" t="s">
+      <c r="D39" s="75"/>
+      <c r="E39" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="90"/>
-      <c r="O39" s="90"/>
-      <c r="P39" s="90"/>
-      <c r="Q39" s="90"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="81"/>
+      <c r="L39" s="81"/>
+      <c r="M39" s="81"/>
+      <c r="N39" s="81"/>
+      <c r="O39" s="81"/>
+      <c r="P39" s="81"/>
+      <c r="Q39" s="81"/>
     </row>
     <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B40" s="88"/>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="D40" s="84"/>
-      <c r="E40" s="91" t="s">
+      <c r="D40" s="76"/>
+      <c r="E40" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="91"/>
-      <c r="L40" s="91"/>
-      <c r="M40" s="91"/>
-      <c r="N40" s="91"/>
-      <c r="O40" s="91"/>
-      <c r="P40" s="91"/>
-      <c r="Q40" s="91"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="89"/>
+      <c r="O40" s="89"/>
+      <c r="P40" s="89"/>
+      <c r="Q40" s="89"/>
     </row>
     <row r="41" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="B41" s="89"/>
-      <c r="C41" s="87" t="s">
+      <c r="B41" s="80"/>
+      <c r="C41" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="D41" s="85"/>
-      <c r="E41" s="90" t="s">
+      <c r="D41" s="77"/>
+      <c r="E41" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
-      <c r="O41" s="90"/>
-      <c r="P41" s="90"/>
-      <c r="Q41" s="90"/>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="81"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="81"/>
+      <c r="O41" s="81"/>
+      <c r="P41" s="81"/>
+      <c r="Q41" s="81"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="81"/>
     </row>
     <row r="42" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="C42" s="87" t="s">
+      <c r="C42" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="86"/>
-      <c r="E42" s="90" t="s">
+      <c r="D42" s="78"/>
+      <c r="E42" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="F42" s="90"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="90"/>
-      <c r="K42" s="90"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="90"/>
-      <c r="N42" s="90"/>
-      <c r="O42" s="90"/>
-      <c r="P42" s="90"/>
-      <c r="Q42" s="90"/>
-      <c r="R42" s="90"/>
-      <c r="S42" s="90"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="81"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="81"/>
+      <c r="L42" s="81"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="81"/>
+      <c r="O42" s="81"/>
+      <c r="P42" s="81"/>
+      <c r="Q42" s="81"/>
+      <c r="R42" s="81"/>
+      <c r="S42" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="E41:S41"/>
-    <mergeCell ref="E42:S42"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:Q39"/>
-    <mergeCell ref="E40:Q40"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="F24:F29"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="F11:F17"/>
     <mergeCell ref="BK4:BL4"/>
     <mergeCell ref="BN4:BO4"/>
     <mergeCell ref="BQ4:BR4"/>
@@ -6747,6 +6749,11 @@
     <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="AM4:AN4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="L4:M4"/>
@@ -6758,18 +6765,14 @@
     <mergeCell ref="AD4:AE4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C11:C17"/>
-    <mergeCell ref="F11:F17"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="F24:F29"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="E41:S41"/>
+    <mergeCell ref="E42:S42"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:Q39"/>
+    <mergeCell ref="E40:Q40"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="36" orientation="landscape" r:id="rId1"/>

</xml_diff>